<commit_message>
BGP,S-1,S-2 Results And Updated data summary statistics
</commit_message>
<xml_diff>
--- a/Data Summary Statistics.xlsx
+++ b/Data Summary Statistics.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="195" windowWidth="20115" windowHeight="7875"/>
+    <workbookView xWindow="240" yWindow="255" windowWidth="20115" windowHeight="7815"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
     <t>Geo Coordinates-2</t>
   </si>
   <si>
-    <t>Geo Coordinates-1</t>
+    <t>Publication</t>
   </si>
 </sst>
 </file>
@@ -116,13 +116,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,7 +429,7 @@
   <dimension ref="A2:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -570,37 +572,41 @@
         <v>3579616</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>2</v>
-      </c>
-      <c r="B9" s="1" t="s">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>4</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="2">
-        <v>274145280</v>
-      </c>
-      <c r="D9" s="2">
-        <v>21981212</v>
-      </c>
-      <c r="E9" s="1">
-        <v>92</v>
-      </c>
-      <c r="F9" s="1">
+      <c r="C6" s="2">
+        <v>39071744</v>
+      </c>
+      <c r="D6" s="2">
+        <v>2784969</v>
+      </c>
+      <c r="E6" s="1">
+        <v>93</v>
+      </c>
+      <c r="F6" s="5">
         <v>10</v>
       </c>
-      <c r="G9" s="1">
-        <v>50000</v>
-      </c>
-      <c r="H9" s="1">
+      <c r="G6" s="5">
+        <v>2500</v>
+      </c>
+      <c r="H6" s="5">
         <v>1</v>
       </c>
-      <c r="I9" s="1">
-        <v>2</v>
-      </c>
-      <c r="J9" s="1">
-        <v>1900006</v>
-      </c>
+      <c r="I6" s="1">
+        <v>10</v>
+      </c>
+      <c r="J6" s="5">
+        <v>234405</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>